<commit_message>
Updated Warrant Modification Response SSP to match elements used in the Warrant Modification Request SSP.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Response/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Response/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1980" windowWidth="25605" windowHeight="15045" tabRatio="500"/>
+    <workbookView xWindow="-26640" yWindow="6860" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Response" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>CLASS</t>
   </si>
@@ -60,30 +60,15 @@
     <t>PERSON</t>
   </si>
   <si>
-    <t>Race Code</t>
-  </si>
-  <si>
-    <t>Sex Code</t>
-  </si>
-  <si>
     <t>ext</t>
   </si>
   <si>
     <t>WARRANT</t>
   </si>
   <si>
-    <t>Law Enforcement ORI</t>
-  </si>
-  <si>
-    <t>Complaint Number</t>
-  </si>
-  <si>
     <t>Person Record Number</t>
   </si>
   <si>
-    <t>ORI of the warrant issuing agency</t>
-  </si>
-  <si>
     <t>The system record number of a person</t>
   </si>
   <si>
@@ -99,20 +84,101 @@
     <t>A unique ID assigned to a modified warrant</t>
   </si>
   <si>
-    <t>Warrant Number</t>
-  </si>
-  <si>
     <t>True if a warrant modification request has been approved; false otherwise</t>
   </si>
   <si>
     <t>Warrant Modification Accepted Indicator</t>
+  </si>
+  <si>
+    <t>Warrant ID</t>
+  </si>
+  <si>
+    <t>Warrant  LE Agency ORI</t>
+  </si>
+  <si>
+    <t>Ext</t>
+  </si>
+  <si>
+    <t>Race Text</t>
+  </si>
+  <si>
+    <t>Sex Text</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Jr</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>PR45789</t>
+  </si>
+  <si>
+    <t>W23345346</t>
+  </si>
+  <si>
+    <t>LE657890</t>
+  </si>
+  <si>
+    <t>W23345346-02</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/j:CourtOrderEnforcementAgency/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/wm-resp-ext:WarrantAugmentation/wm-resp-ext:PersonRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/wm-resp-ext:WarrantAugmentation/wm-resp-ext:WarrantModificationAcceptedIndicator</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/wm-resp-ext:WarrantAugmentation/wm-resp-ext:ModifiedWarrantNumber/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/wm-resp-ext:PersonRecordIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,12 +253,6 @@
       <sz val="11"/>
       <name val="Verdana"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF6600"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -228,7 +288,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="786">
+  <cellStyleXfs count="798">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1015,8 +1075,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1063,13 +1135,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,11 +1147,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="786">
+  <cellStyles count="798">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1478,6 +1553,12 @@
     <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1870,6 +1951,12 @@
     <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2205,38 +2292,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G335"/>
+  <dimension ref="A1:G334"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="92.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="12"/>
-      <c r="B1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="23"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -2257,1870 +2344,1924 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="16"/>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="22">
+        <v>23235</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1">
+      <c r="A9" s="16"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="30">
+      <c r="A11" s="16"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="16"/>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" s="18" customFormat="1">
+      <c r="A13" s="11"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="21" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" s="18" customFormat="1" ht="45">
+      <c r="A14" s="11"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" s="18" customFormat="1" ht="30">
+      <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="11" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" s="18" customFormat="1" ht="30">
+      <c r="A16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" s="18" customFormat="1" ht="30">
+      <c r="A17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="D17" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="E17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1">
+      <c r="A18" s="16"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="C18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:7" s="13" customFormat="1">
+      <c r="A19" s="16"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:7" s="13" customFormat="1">
+      <c r="A20" s="16"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+    <row r="21" spans="1:7" s="13" customFormat="1">
+      <c r="A21" s="16"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+    <row r="22" spans="1:7" s="13" customFormat="1">
+      <c r="A22" s="16"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:7" s="13" customFormat="1">
+      <c r="A23" s="16"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="16"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:7">
+      <c r="A26" s="16"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:7">
+      <c r="A27" s="16"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:7">
+      <c r="A28" s="16"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+    <row r="29" spans="1:7">
+      <c r="A29" s="16"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+    <row r="30" spans="1:7">
+      <c r="A30" s="16"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+    <row r="31" spans="1:7">
+      <c r="A31" s="16"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
+    <row r="32" spans="1:7">
+      <c r="A32" s="16"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
+    <row r="33" spans="1:6">
+      <c r="A33" s="16"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
+    <row r="34" spans="1:6">
+      <c r="A34" s="16"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
+    <row r="35" spans="1:6">
+      <c r="A35" s="16"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
+    <row r="36" spans="1:6">
+      <c r="A36" s="16"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+    <row r="37" spans="1:6">
+      <c r="A37" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>15</v>
+    <row r="38" spans="1:6">
+      <c r="A38" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>15</v>
+    <row r="39" spans="1:6">
+      <c r="A39" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>15</v>
+    <row r="40" spans="1:6">
+      <c r="A40" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>15</v>
-      </c>
+    <row r="41" spans="1:6">
+      <c r="A41" s="16"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
+    <row r="42" spans="1:6">
+      <c r="A42" s="16"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
+    <row r="43" spans="1:6">
+      <c r="A43" s="16"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
+    <row r="44" spans="1:6">
+      <c r="A44" s="16"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
+    <row r="45" spans="1:6">
+      <c r="A45" s="16"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
+    <row r="46" spans="1:6">
+      <c r="A46" s="16"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
+    <row r="47" spans="1:6">
+      <c r="A47" s="16"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+    <row r="48" spans="1:6">
+      <c r="A48" s="16"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
+    <row r="49" spans="1:6">
+      <c r="A49" s="16"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
+    <row r="50" spans="1:6">
+      <c r="A50" s="16"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
+    <row r="51" spans="1:6">
+      <c r="A51" s="16"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
+    <row r="52" spans="1:6">
+      <c r="A52" s="16"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
+    <row r="53" spans="1:6">
+      <c r="A53" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
-        <v>15</v>
+    <row r="54" spans="1:6">
+      <c r="A54" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="F54" s="8"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>15</v>
+    <row r="55" spans="1:6">
+      <c r="A55" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="F55" s="8"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>15</v>
-      </c>
+    <row r="56" spans="1:6">
+      <c r="A56" s="16"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="F56" s="8"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
+    <row r="57" spans="1:6">
+      <c r="A57" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="F57" s="8"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>15</v>
-      </c>
+    <row r="58" spans="1:6">
+      <c r="A58" s="11"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="F58" s="8"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="11"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
+    <row r="60" spans="1:6">
+      <c r="A60" s="16"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
+    <row r="61" spans="1:6">
+      <c r="A61" s="16"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="F61" s="8"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
+    <row r="62" spans="1:6">
+      <c r="A62" s="16"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="F62" s="8"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
+    <row r="63" spans="1:6">
+      <c r="A63" s="16"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="F63" s="8"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
+    <row r="64" spans="1:6">
+      <c r="A64" s="16"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="F64" s="8"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
+    <row r="65" spans="1:6">
+      <c r="A65" s="16"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="F65" s="8"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
+    <row r="66" spans="1:6">
+      <c r="A66" s="16"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="F66" s="8"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
+    <row r="67" spans="1:6">
+      <c r="A67" s="16"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="F67" s="8"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
+    <row r="68" spans="1:6">
+      <c r="A68" s="16"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="F68" s="8"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
+    <row r="69" spans="1:6">
+      <c r="A69" s="16"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
+    <row r="70" spans="1:6">
+      <c r="A70" s="16"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
+    <row r="71" spans="1:6">
+      <c r="A71" s="16"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
       <c r="F71" s="8"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
+    <row r="72" spans="1:6">
+      <c r="A72" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>15</v>
+    <row r="73" spans="1:6">
+      <c r="A73" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="F73" s="8"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>15</v>
-      </c>
+    <row r="74" spans="1:6">
+      <c r="A74" s="16"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
       <c r="F74" s="8"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
+    <row r="75" spans="1:6">
+      <c r="A75" s="16"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
       <c r="F75" s="8"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
+    <row r="76" spans="1:6">
+      <c r="A76" s="16"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="F76" s="8"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
+    <row r="77" spans="1:6">
+      <c r="A77" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
       <c r="F77" s="8"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>15</v>
+    <row r="78" spans="1:6">
+      <c r="A78" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
       <c r="F78" s="8"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>15</v>
+    <row r="79" spans="1:6">
+      <c r="A79" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
       <c r="F79" s="8"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>15</v>
+    <row r="80" spans="1:6">
+      <c r="A80" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>15</v>
-      </c>
+    <row r="81" spans="1:6">
+      <c r="A81" s="16"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
       <c r="F81" s="8"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
+    <row r="82" spans="1:6">
+      <c r="A82" s="16"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
       <c r="F82" s="8"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
+    <row r="83" spans="1:6">
+      <c r="A83" s="16"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
       <c r="F83" s="8"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
+    <row r="84" spans="1:6">
+      <c r="A84" s="16"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
       <c r="F84" s="8"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
+    <row r="85" spans="1:6">
+      <c r="A85" s="16"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
       <c r="F85" s="8"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
+    <row r="86" spans="1:6">
+      <c r="A86" s="16"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="F86" s="8"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
+    <row r="87" spans="1:6">
+      <c r="A87" s="16"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="F87" s="8"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
+    <row r="88" spans="1:6">
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
       <c r="F88" s="8"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
       <c r="F89" s="8"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
       <c r="F90" s="8"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
       <c r="F91" s="8"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="F92" s="8"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
       <c r="F93" s="8"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
       <c r="F94" s="8"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
       <c r="F95" s="8"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
       <c r="F96" s="8"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6">
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
       <c r="F97" s="8"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6">
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
       <c r="F98" s="8"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6">
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
       <c r="F99" s="8"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6">
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
       <c r="F100" s="8"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6">
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="F101" s="8"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6">
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="F102" s="8"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6">
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="F103" s="8"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6">
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
       <c r="F104" s="8"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6">
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
       <c r="F105" s="8"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6">
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
       <c r="F106" s="8"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6">
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
       <c r="F107" s="8"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6">
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
       <c r="F108" s="8"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6">
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="F109" s="8"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6">
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
       <c r="F110" s="8"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6">
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
       <c r="F111" s="8"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6">
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
       <c r="F112" s="8"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6">
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
       <c r="F113" s="8"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6">
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
       <c r="F114" s="8"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6">
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
       <c r="F115" s="8"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6">
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
       <c r="F116" s="8"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6">
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
       <c r="F117" s="8"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6">
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
       <c r="F118" s="8"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6">
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
       <c r="F119" s="8"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6">
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
       <c r="F120" s="8"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6">
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="F121" s="8"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6">
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
       <c r="F122" s="8"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6">
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
       <c r="F123" s="8"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6">
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="F124" s="8"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6">
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
       <c r="F125" s="8"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6">
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
       <c r="F126" s="8"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6">
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="F127" s="8"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6">
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
       <c r="F128" s="8"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:6">
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="F129" s="8"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:6">
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
       <c r="F130" s="8"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6">
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
       <c r="F131" s="8"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6">
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
       <c r="F132" s="8"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:6">
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
       <c r="F133" s="8"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6">
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="F134" s="8"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6">
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="F135" s="8"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:6">
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
       <c r="F136" s="8"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6">
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
       <c r="F137" s="8"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:6">
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
       <c r="F138" s="8"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:6">
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
       <c r="F139" s="8"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6">
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
       <c r="F140" s="8"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6">
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
       <c r="F141" s="8"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:6">
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="F142" s="8"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6">
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
       <c r="F143" s="8"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6">
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
       <c r="F144" s="8"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6">
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
       <c r="F145" s="8"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:6">
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
       <c r="F146" s="8"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6">
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
       <c r="F147" s="8"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:6">
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
       <c r="F148" s="8"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:6">
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
       <c r="F149" s="8"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:6">
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
       <c r="F150" s="8"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:6">
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
       <c r="F151" s="8"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:6">
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
       <c r="F152" s="8"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:6">
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
       <c r="F153" s="8"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:6">
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
       <c r="F154" s="8"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:6">
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
       <c r="F155" s="8"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:6">
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="F156" s="8"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:6">
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
       <c r="F157" s="8"/>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:6">
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
       <c r="F158" s="8"/>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:6">
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
       <c r="F159" s="8"/>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:6">
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="F160" s="8"/>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:6">
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
       <c r="F161" s="8"/>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:6">
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
       <c r="F162" s="8"/>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:6">
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
       <c r="F163" s="8"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:6">
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
       <c r="F164" s="8"/>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:6">
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
       <c r="F165" s="8"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:6">
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
       <c r="F166" s="8"/>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6">
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
       <c r="F167" s="8"/>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:6">
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
       <c r="F168" s="8"/>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:6">
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
       <c r="F169" s="8"/>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:6">
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
       <c r="F170" s="8"/>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:6">
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
       <c r="F171" s="8"/>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:6">
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
       <c r="F172" s="8"/>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:6">
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
       <c r="F173" s="8"/>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:6">
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
       <c r="F174" s="8"/>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:6">
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
       <c r="F175" s="8"/>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:6">
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
       <c r="F176" s="8"/>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:6">
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
       <c r="F177" s="8"/>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:6">
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
       <c r="F178" s="8"/>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:6">
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
       <c r="F179" s="8"/>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:6">
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
       <c r="F180" s="8"/>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:6">
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
       <c r="F181" s="8"/>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:6">
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
       <c r="F182" s="8"/>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:6">
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
       <c r="F183" s="8"/>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:6">
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
       <c r="F184" s="8"/>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:6">
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
       <c r="F185" s="8"/>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:6">
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
       <c r="F186" s="8"/>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:6">
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
       <c r="F187" s="8"/>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:6">
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
       <c r="F188" s="8"/>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:6">
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
       <c r="F189" s="8"/>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:6">
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
       <c r="F190" s="8"/>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:6">
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
       <c r="F191" s="8"/>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:6">
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
       <c r="F192" s="8"/>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:6">
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
       <c r="F193" s="8"/>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:6">
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
       <c r="F194" s="8"/>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:6">
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
       <c r="F195" s="8"/>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:6">
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
       <c r="F196" s="8"/>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:6">
       <c r="B197" s="8"/>
       <c r="C197" s="8"/>
       <c r="F197" s="8"/>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:6">
       <c r="B198" s="8"/>
       <c r="C198" s="8"/>
       <c r="F198" s="8"/>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:6">
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
       <c r="F199" s="8"/>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:6">
       <c r="B200" s="8"/>
       <c r="C200" s="8"/>
       <c r="F200" s="8"/>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:6">
       <c r="B201" s="8"/>
       <c r="C201" s="8"/>
       <c r="F201" s="8"/>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:6">
       <c r="B202" s="8"/>
       <c r="C202" s="8"/>
       <c r="F202" s="8"/>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:6">
       <c r="B203" s="8"/>
       <c r="C203" s="8"/>
       <c r="F203" s="8"/>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:6">
       <c r="B204" s="8"/>
       <c r="C204" s="8"/>
       <c r="F204" s="8"/>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:6">
       <c r="B205" s="8"/>
       <c r="C205" s="8"/>
       <c r="F205" s="8"/>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:6">
       <c r="B206" s="8"/>
       <c r="C206" s="8"/>
       <c r="F206" s="8"/>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:6">
       <c r="B207" s="8"/>
       <c r="C207" s="8"/>
       <c r="F207" s="8"/>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:6">
       <c r="B208" s="8"/>
       <c r="C208" s="8"/>
       <c r="F208" s="8"/>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:6">
       <c r="B209" s="8"/>
       <c r="C209" s="8"/>
       <c r="F209" s="8"/>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:6">
       <c r="B210" s="8"/>
       <c r="C210" s="8"/>
       <c r="F210" s="8"/>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:6">
       <c r="B211" s="8"/>
       <c r="C211" s="8"/>
       <c r="F211" s="8"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:6">
       <c r="B212" s="8"/>
       <c r="C212" s="8"/>
       <c r="F212" s="8"/>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:6">
       <c r="B213" s="8"/>
       <c r="C213" s="8"/>
       <c r="F213" s="8"/>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:6">
       <c r="B214" s="8"/>
       <c r="C214" s="8"/>
       <c r="F214" s="8"/>
     </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:6">
       <c r="B215" s="8"/>
       <c r="C215" s="8"/>
       <c r="F215" s="8"/>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:6">
       <c r="B216" s="8"/>
       <c r="C216" s="8"/>
       <c r="F216" s="8"/>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:6">
       <c r="B217" s="8"/>
       <c r="C217" s="8"/>
       <c r="F217" s="8"/>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:6">
       <c r="B218" s="8"/>
       <c r="C218" s="8"/>
       <c r="F218" s="8"/>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:6">
       <c r="B219" s="8"/>
       <c r="C219" s="8"/>
       <c r="F219" s="8"/>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:6">
       <c r="B220" s="8"/>
       <c r="C220" s="8"/>
       <c r="F220" s="8"/>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:6">
       <c r="B221" s="8"/>
       <c r="C221" s="8"/>
       <c r="F221" s="8"/>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:6">
       <c r="B222" s="8"/>
       <c r="C222" s="8"/>
       <c r="F222" s="8"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:6">
       <c r="B223" s="8"/>
       <c r="C223" s="8"/>
       <c r="F223" s="8"/>
     </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:6">
       <c r="B224" s="8"/>
       <c r="C224" s="8"/>
       <c r="F224" s="8"/>
     </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:6">
       <c r="B225" s="8"/>
       <c r="C225" s="8"/>
       <c r="F225" s="8"/>
     </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:6">
       <c r="B226" s="8"/>
       <c r="C226" s="8"/>
       <c r="F226" s="8"/>
     </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:6">
       <c r="B227" s="8"/>
       <c r="C227" s="8"/>
       <c r="F227" s="8"/>
     </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:6">
       <c r="B228" s="8"/>
       <c r="C228" s="8"/>
       <c r="F228" s="8"/>
     </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:6">
       <c r="B229" s="8"/>
       <c r="C229" s="8"/>
       <c r="F229" s="8"/>
     </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:6">
       <c r="B230" s="8"/>
       <c r="C230" s="8"/>
       <c r="F230" s="8"/>
     </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:6">
       <c r="B231" s="8"/>
       <c r="C231" s="8"/>
       <c r="F231" s="8"/>
     </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:6">
       <c r="B232" s="8"/>
       <c r="C232" s="8"/>
       <c r="F232" s="8"/>
     </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:6">
       <c r="B233" s="8"/>
       <c r="C233" s="8"/>
       <c r="F233" s="8"/>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:6">
       <c r="B234" s="8"/>
       <c r="C234" s="8"/>
       <c r="F234" s="8"/>
     </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:6">
       <c r="B235" s="8"/>
       <c r="C235" s="8"/>
       <c r="F235" s="8"/>
     </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:6">
       <c r="B236" s="8"/>
       <c r="C236" s="8"/>
       <c r="F236" s="8"/>
     </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:6">
       <c r="B237" s="8"/>
       <c r="C237" s="8"/>
       <c r="F237" s="8"/>
     </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:6">
       <c r="B238" s="8"/>
       <c r="C238" s="8"/>
       <c r="F238" s="8"/>
     </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:6">
       <c r="B239" s="8"/>
       <c r="C239" s="8"/>
       <c r="F239" s="8"/>
     </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:6">
       <c r="B240" s="8"/>
       <c r="C240" s="8"/>
       <c r="F240" s="8"/>
     </row>
-    <row r="241" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:6">
       <c r="B241" s="8"/>
       <c r="C241" s="8"/>
       <c r="F241" s="8"/>
     </row>
-    <row r="242" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:6">
       <c r="B242" s="8"/>
       <c r="C242" s="8"/>
       <c r="F242" s="8"/>
     </row>
-    <row r="243" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:6">
       <c r="B243" s="8"/>
       <c r="C243" s="8"/>
       <c r="F243" s="8"/>
     </row>
-    <row r="244" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:6">
       <c r="B244" s="8"/>
       <c r="C244" s="8"/>
       <c r="F244" s="8"/>
     </row>
-    <row r="245" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:6">
       <c r="B245" s="8"/>
       <c r="C245" s="8"/>
       <c r="F245" s="8"/>
     </row>
-    <row r="246" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:6">
       <c r="B246" s="8"/>
       <c r="C246" s="8"/>
       <c r="F246" s="8"/>
     </row>
-    <row r="247" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:6">
       <c r="B247" s="8"/>
       <c r="C247" s="8"/>
       <c r="F247" s="8"/>
     </row>
-    <row r="248" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:6">
       <c r="B248" s="8"/>
       <c r="C248" s="8"/>
       <c r="F248" s="8"/>
     </row>
-    <row r="249" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:6">
       <c r="B249" s="8"/>
       <c r="C249" s="8"/>
       <c r="F249" s="8"/>
     </row>
-    <row r="250" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:6">
       <c r="B250" s="8"/>
       <c r="C250" s="8"/>
       <c r="F250" s="8"/>
     </row>
-    <row r="251" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:6">
       <c r="B251" s="8"/>
       <c r="C251" s="8"/>
       <c r="F251" s="8"/>
     </row>
-    <row r="252" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:6">
       <c r="B252" s="8"/>
       <c r="C252" s="8"/>
       <c r="F252" s="8"/>
     </row>
-    <row r="253" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:6">
       <c r="B253" s="8"/>
       <c r="C253" s="8"/>
       <c r="F253" s="8"/>
     </row>
-    <row r="254" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:6">
       <c r="B254" s="8"/>
       <c r="C254" s="8"/>
       <c r="F254" s="8"/>
     </row>
-    <row r="255" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:6">
       <c r="B255" s="8"/>
       <c r="C255" s="8"/>
       <c r="F255" s="8"/>
     </row>
-    <row r="256" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:6">
       <c r="B256" s="8"/>
       <c r="C256" s="8"/>
       <c r="F256" s="8"/>
     </row>
-    <row r="257" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:6">
       <c r="B257" s="8"/>
       <c r="C257" s="8"/>
       <c r="F257" s="8"/>
     </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:6">
       <c r="B258" s="8"/>
       <c r="C258" s="8"/>
       <c r="F258" s="8"/>
     </row>
-    <row r="259" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:6">
       <c r="B259" s="8"/>
       <c r="C259" s="8"/>
       <c r="F259" s="8"/>
     </row>
-    <row r="260" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:6">
       <c r="B260" s="8"/>
       <c r="C260" s="8"/>
       <c r="F260" s="8"/>
     </row>
-    <row r="261" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:6">
       <c r="B261" s="8"/>
       <c r="C261" s="8"/>
       <c r="F261" s="8"/>
     </row>
-    <row r="262" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:6">
       <c r="B262" s="8"/>
       <c r="C262" s="8"/>
       <c r="F262" s="8"/>
     </row>
-    <row r="263" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:6">
       <c r="B263" s="8"/>
       <c r="C263" s="8"/>
       <c r="F263" s="8"/>
     </row>
-    <row r="264" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:6">
       <c r="B264" s="8"/>
       <c r="C264" s="8"/>
       <c r="F264" s="8"/>
     </row>
-    <row r="265" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:6">
       <c r="B265" s="8"/>
       <c r="C265" s="8"/>
       <c r="F265" s="8"/>
     </row>
-    <row r="266" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:6">
       <c r="B266" s="8"/>
       <c r="C266" s="8"/>
       <c r="F266" s="8"/>
     </row>
-    <row r="267" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:6">
       <c r="B267" s="8"/>
       <c r="C267" s="8"/>
       <c r="F267" s="8"/>
     </row>
-    <row r="268" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:6">
       <c r="B268" s="8"/>
       <c r="C268" s="8"/>
       <c r="F268" s="8"/>
     </row>
-    <row r="269" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:6">
       <c r="B269" s="8"/>
       <c r="C269" s="8"/>
       <c r="F269" s="8"/>
     </row>
-    <row r="270" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:6">
       <c r="B270" s="8"/>
       <c r="C270" s="8"/>
       <c r="F270" s="8"/>
     </row>
-    <row r="271" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:6">
       <c r="B271" s="8"/>
       <c r="C271" s="8"/>
       <c r="F271" s="8"/>
     </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:6">
       <c r="B272" s="8"/>
       <c r="C272" s="8"/>
       <c r="F272" s="8"/>
     </row>
-    <row r="273" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:6">
       <c r="B273" s="8"/>
       <c r="C273" s="8"/>
       <c r="F273" s="8"/>
     </row>
-    <row r="274" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:6">
       <c r="B274" s="8"/>
       <c r="C274" s="8"/>
       <c r="F274" s="8"/>
     </row>
-    <row r="275" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:6">
       <c r="B275" s="8"/>
       <c r="C275" s="8"/>
       <c r="F275" s="8"/>
     </row>
-    <row r="276" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:6">
       <c r="B276" s="8"/>
       <c r="C276" s="8"/>
       <c r="F276" s="8"/>
     </row>
-    <row r="277" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:6">
       <c r="B277" s="8"/>
       <c r="C277" s="8"/>
       <c r="F277" s="8"/>
     </row>
-    <row r="278" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:6">
       <c r="B278" s="8"/>
       <c r="C278" s="8"/>
       <c r="F278" s="8"/>
     </row>
-    <row r="279" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:6">
       <c r="B279" s="8"/>
       <c r="C279" s="8"/>
       <c r="F279" s="8"/>
     </row>
-    <row r="280" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:6">
       <c r="B280" s="8"/>
       <c r="C280" s="8"/>
       <c r="F280" s="8"/>
     </row>
-    <row r="281" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:6">
       <c r="B281" s="8"/>
       <c r="C281" s="8"/>
       <c r="F281" s="8"/>
     </row>
-    <row r="282" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:6">
       <c r="B282" s="8"/>
       <c r="C282" s="8"/>
       <c r="F282" s="8"/>
     </row>
-    <row r="283" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:6">
       <c r="B283" s="8"/>
       <c r="C283" s="8"/>
       <c r="F283" s="8"/>
     </row>
-    <row r="284" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:6">
       <c r="B284" s="8"/>
       <c r="C284" s="8"/>
       <c r="F284" s="8"/>
     </row>
-    <row r="285" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:6">
       <c r="B285" s="8"/>
       <c r="C285" s="8"/>
       <c r="F285" s="8"/>
     </row>
-    <row r="286" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:6">
       <c r="B286" s="8"/>
       <c r="C286" s="8"/>
       <c r="F286" s="8"/>
     </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:6">
       <c r="B287" s="8"/>
       <c r="C287" s="8"/>
       <c r="F287" s="8"/>
     </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:6">
       <c r="B288" s="8"/>
       <c r="C288" s="8"/>
       <c r="F288" s="8"/>
     </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:6">
       <c r="B289" s="8"/>
       <c r="C289" s="8"/>
       <c r="F289" s="8"/>
     </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:6">
       <c r="B290" s="8"/>
       <c r="C290" s="8"/>
       <c r="F290" s="8"/>
     </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:6">
       <c r="B291" s="8"/>
       <c r="C291" s="8"/>
       <c r="F291" s="8"/>
     </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:6">
       <c r="B292" s="8"/>
       <c r="C292" s="8"/>
       <c r="F292" s="8"/>
     </row>
-    <row r="293" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:6">
       <c r="B293" s="8"/>
       <c r="C293" s="8"/>
       <c r="F293" s="8"/>
     </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:6">
       <c r="B294" s="8"/>
       <c r="C294" s="8"/>
       <c r="F294" s="8"/>
     </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:6">
       <c r="B295" s="8"/>
       <c r="C295" s="8"/>
       <c r="F295" s="8"/>
     </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:6">
       <c r="B296" s="8"/>
       <c r="C296" s="8"/>
       <c r="F296" s="8"/>
     </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:6">
       <c r="B297" s="8"/>
       <c r="C297" s="8"/>
       <c r="F297" s="8"/>
     </row>
-    <row r="298" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:6">
       <c r="B298" s="8"/>
       <c r="C298" s="8"/>
       <c r="F298" s="8"/>
     </row>
-    <row r="299" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:6">
       <c r="B299" s="8"/>
       <c r="C299" s="8"/>
       <c r="F299" s="8"/>
     </row>
-    <row r="300" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:6">
       <c r="B300" s="8"/>
       <c r="C300" s="8"/>
       <c r="F300" s="8"/>
     </row>
-    <row r="301" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:6">
       <c r="B301" s="8"/>
       <c r="C301" s="8"/>
       <c r="F301" s="8"/>
     </row>
-    <row r="302" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:6">
       <c r="B302" s="8"/>
       <c r="C302" s="8"/>
       <c r="F302" s="8"/>
     </row>
-    <row r="303" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:6">
       <c r="B303" s="8"/>
       <c r="C303" s="8"/>
       <c r="F303" s="8"/>
     </row>
-    <row r="304" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:6">
       <c r="B304" s="8"/>
       <c r="C304" s="8"/>
       <c r="F304" s="8"/>
     </row>
-    <row r="305" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:6">
       <c r="B305" s="8"/>
       <c r="C305" s="8"/>
       <c r="F305" s="8"/>
     </row>
-    <row r="306" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:6">
       <c r="B306" s="8"/>
       <c r="C306" s="8"/>
       <c r="F306" s="8"/>
     </row>
-    <row r="307" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:6">
       <c r="B307" s="8"/>
       <c r="C307" s="8"/>
       <c r="F307" s="8"/>
     </row>
-    <row r="308" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:6">
       <c r="B308" s="8"/>
       <c r="C308" s="8"/>
       <c r="F308" s="8"/>
     </row>
-    <row r="309" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:6">
       <c r="B309" s="8"/>
       <c r="C309" s="8"/>
       <c r="F309" s="8"/>
     </row>
-    <row r="310" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:6">
       <c r="B310" s="8"/>
       <c r="C310" s="8"/>
       <c r="F310" s="8"/>
     </row>
-    <row r="311" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:6">
       <c r="B311" s="8"/>
       <c r="C311" s="8"/>
       <c r="F311" s="8"/>
     </row>
-    <row r="312" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:6">
       <c r="B312" s="8"/>
       <c r="C312" s="8"/>
       <c r="F312" s="8"/>
     </row>
-    <row r="313" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:6">
       <c r="B313" s="8"/>
       <c r="C313" s="8"/>
       <c r="F313" s="8"/>
     </row>
-    <row r="314" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:6">
       <c r="B314" s="8"/>
       <c r="C314" s="8"/>
       <c r="F314" s="8"/>
     </row>
-    <row r="315" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:6">
       <c r="B315" s="8"/>
       <c r="C315" s="8"/>
       <c r="F315" s="8"/>
     </row>
-    <row r="316" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:6">
       <c r="B316" s="8"/>
       <c r="C316" s="8"/>
       <c r="F316" s="8"/>
     </row>
-    <row r="317" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:6">
       <c r="B317" s="8"/>
       <c r="C317" s="8"/>
       <c r="F317" s="8"/>
     </row>
-    <row r="318" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:6">
       <c r="B318" s="8"/>
       <c r="C318" s="8"/>
       <c r="F318" s="8"/>
     </row>
-    <row r="319" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:6">
       <c r="B319" s="8"/>
       <c r="C319" s="8"/>
       <c r="F319" s="8"/>
     </row>
-    <row r="320" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:6">
       <c r="B320" s="8"/>
       <c r="C320" s="8"/>
       <c r="F320" s="8"/>
     </row>
-    <row r="321" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:6">
       <c r="B321" s="8"/>
       <c r="C321" s="8"/>
       <c r="F321" s="8"/>
     </row>
-    <row r="322" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:6">
       <c r="B322" s="8"/>
       <c r="C322" s="8"/>
       <c r="F322" s="8"/>
     </row>
-    <row r="323" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:6">
       <c r="B323" s="8"/>
       <c r="C323" s="8"/>
       <c r="F323" s="8"/>
     </row>
-    <row r="324" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:6">
       <c r="B324" s="8"/>
       <c r="C324" s="8"/>
       <c r="F324" s="8"/>
     </row>
-    <row r="325" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:6">
       <c r="B325" s="8"/>
       <c r="C325" s="8"/>
       <c r="F325" s="8"/>
     </row>
-    <row r="326" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:6">
       <c r="B326" s="8"/>
       <c r="C326" s="8"/>
       <c r="F326" s="8"/>
     </row>
-    <row r="327" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:6">
       <c r="B327" s="8"/>
       <c r="C327" s="8"/>
       <c r="F327" s="8"/>
     </row>
-    <row r="328" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:6">
       <c r="B328" s="8"/>
       <c r="C328" s="8"/>
       <c r="F328" s="8"/>
     </row>
-    <row r="329" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:6">
       <c r="B329" s="8"/>
       <c r="C329" s="8"/>
       <c r="F329" s="8"/>
     </row>
-    <row r="330" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:6">
       <c r="B330" s="8"/>
       <c r="C330" s="8"/>
       <c r="F330" s="8"/>
     </row>
-    <row r="331" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:6">
       <c r="B331" s="8"/>
       <c r="C331" s="8"/>
       <c r="F331" s="8"/>
     </row>
-    <row r="332" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:6">
       <c r="B332" s="8"/>
       <c r="C332" s="8"/>
       <c r="F332" s="8"/>
     </row>
-    <row r="333" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:6">
       <c r="B333" s="8"/>
       <c r="C333" s="8"/>
       <c r="F333" s="8"/>
     </row>
-    <row r="334" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:6">
       <c r="B334" s="8"/>
       <c r="C334" s="8"/>
       <c r="F334" s="8"/>
-    </row>
-    <row r="335" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B335" s="8"/>
-      <c r="C335" s="8"/>
-      <c r="F335" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Replaced "Person Record Identification ID” in the Warrant Modification Request” with "State Warrant Repository ID”.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Response/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Response/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26640" yWindow="6860" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="7740" yWindow="2940" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Response" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>CLASS</t>
   </si>
@@ -66,12 +66,6 @@
     <t>WARRANT</t>
   </si>
   <si>
-    <t>Person Record Number</t>
-  </si>
-  <si>
-    <t>The system record number of a person</t>
-  </si>
-  <si>
     <t>EXTENSION ?</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>PR45789</t>
-  </si>
-  <si>
     <t>W23345346</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/j:CourtOrderEnforcementAgency/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/wm-resp-ext:WarrantAugmentation/wm-resp-ext:PersonRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/wm-resp-ext:WarrantAugmentation/wm-resp-ext:WarrantModificationAcceptedIndicator</t>
   </si>
   <si>
@@ -171,7 +159,16 @@
     <t>wm-resp-doc:WarrantModificationResponse/nc:Person/nc:PersonSexText</t>
   </si>
   <si>
-    <t>wm-resp-doc:WarrantModificationResponse/nc:Person/wm-resp-ext:PersonRecordIdentification/nc:IdentificationID</t>
+    <t>State Warrant Repository ID</t>
+  </si>
+  <si>
+    <t>A unique identification assigned to a warrant record.</t>
+  </si>
+  <si>
+    <t>PE45678</t>
+  </si>
+  <si>
+    <t>wm-resp-doc:WarrantModificationResponse/j:Warrant/wm-resp-ext:WarrantAugmentation/wm-resp-ext:StateWarrantRepositoryIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -2292,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G334"/>
+  <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2313,7 +2310,7 @@
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="12"/>
       <c r="B1" s="23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="12"/>
@@ -2323,7 +2320,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -2365,10 +2362,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1">
@@ -2379,10 +2376,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1">
@@ -2393,10 +2390,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1">
@@ -2407,10 +2404,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1">
@@ -2424,7 +2421,7 @@
         <v>23235</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G8" s="11"/>
     </row>
@@ -2432,14 +2429,14 @@
       <c r="A9" s="16"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G9" s="11"/>
     </row>
@@ -2447,217 +2444,206 @@
       <c r="A10" s="16"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="30">
+    <row r="11" spans="1:7">
       <c r="A11" s="16"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="16"/>
-      <c r="B12" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" s="18" customFormat="1">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" s="18" customFormat="1">
+      <c r="A12" s="11"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" s="18" customFormat="1" ht="45">
       <c r="A13" s="11"/>
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" s="18" customFormat="1" ht="45">
-      <c r="A14" s="11"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>39</v>
+    <row r="14" spans="1:7" s="18" customFormat="1" ht="30">
+      <c r="A14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" s="18" customFormat="1" ht="30">
       <c r="A15" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="17"/>
-      <c r="C15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>34</v>
+      <c r="C15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="20" t="b">
+        <v>1</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:7" s="18" customFormat="1" ht="30">
       <c r="A16" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="20" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" s="18" customFormat="1" ht="30">
-      <c r="A17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="1:7" s="13" customFormat="1">
+    <row r="17" spans="1:6" s="13" customFormat="1">
+      <c r="A17" s="16"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" s="13" customFormat="1">
       <c r="A18" s="16"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1">
+    <row r="19" spans="1:6" s="13" customFormat="1">
       <c r="A19" s="16"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1">
+    <row r="20" spans="1:6" s="13" customFormat="1">
       <c r="A20" s="16"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1">
+    <row r="21" spans="1:6" s="13" customFormat="1">
       <c r="A21" s="16"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1">
+    <row r="22" spans="1:6" s="13" customFormat="1">
       <c r="A22" s="16"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:7" s="13" customFormat="1">
+    <row r="23" spans="1:6">
       <c r="A23" s="16"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="16"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:6">
       <c r="A25" s="16"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:6">
       <c r="A26" s="16"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:6">
       <c r="A27" s="16"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:6">
       <c r="A28" s="16"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:6">
       <c r="A29" s="16"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:6">
       <c r="A30" s="16"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:6">
       <c r="A31" s="16"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:6">
       <c r="A32" s="16"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2682,7 +2668,9 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="16"/>
+      <c r="A36" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="F36" s="8"/>
@@ -2712,9 +2700,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A40" s="16"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="F40" s="8"/>
@@ -2786,7 +2772,9 @@
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="16"/>
+      <c r="A52" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="F52" s="8"/>
@@ -2808,23 +2796,21 @@
       <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A55" s="16"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="16"/>
+      <c r="A56" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="F56" s="8"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="A57" s="11"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="F57" s="8"/>
@@ -2836,7 +2822,7 @@
       <c r="F58" s="8"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="11"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="F59" s="8"/>
@@ -2908,7 +2894,9 @@
       <c r="F70" s="8"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="16"/>
+      <c r="A71" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
       <c r="F71" s="8"/>
@@ -2922,9 +2910,7 @@
       <c r="F72" s="8"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A73" s="16"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="F73" s="8"/>
@@ -2942,7 +2928,9 @@
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="16"/>
+      <c r="A76" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="F76" s="8"/>
@@ -2972,9 +2960,7 @@
       <c r="F79" s="8"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A80" s="16"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="F80" s="8"/>
@@ -3016,7 +3002,6 @@
       <c r="F86" s="8"/>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="16"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="F87" s="8"/>
@@ -4250,11 +4235,6 @@
       <c r="B333" s="8"/>
       <c r="C333" s="8"/>
       <c r="F333" s="8"/>
-    </row>
-    <row r="334" spans="2:6">
-      <c r="B334" s="8"/>
-      <c r="C334" s="8"/>
-      <c r="F334" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>